<commit_message>
1. improved comments 2. Stopped browser from opening 3. made error handling more clear
</commit_message>
<xml_diff>
--- a/output_list.xlsx
+++ b/output_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nithin\Desktop\CpTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2E090D-036E-44F4-A6EF-F124A75F55B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC34D8-6C1D-4B16-8B43-0502CD810BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,42 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>['Nithin_XS1223']</t>
+  </si>
+  <si>
+    <t>INVALID USER</t>
+  </si>
   <si>
     <t>['Radewoosh']</t>
   </si>
   <si>
-    <t>3759</t>
-  </si>
-  <si>
     <t>['orzdevinwang']</t>
   </si>
   <si>
-    <t>3697</t>
-  </si>
-  <si>
     <t>['jiangly']</t>
   </si>
   <si>
-    <t>3662</t>
-  </si>
-  <si>
     <t>['Benq']</t>
   </si>
   <si>
-    <t>3644</t>
-  </si>
-  <si>
     <t>['ecnerwala']</t>
   </si>
   <si>
-    <t>3505</t>
-  </si>
-  <si>
     <t>['tourist']</t>
-  </si>
-  <si>
-    <t>3486</t>
   </si>
 </sst>
 </file>
@@ -96,11 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,14 +392,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -433,40 +424,48 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="B4" s="2">
+        <v>3759</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3697</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3662</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3644</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>